<commit_message>
second commit - deleted some reports and added some validations
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2448" windowWidth="19272" windowHeight="4572" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="2448" windowWidth="19272" windowHeight="4428" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,9 @@
     <sheet name="addCustomer" sheetId="4" r:id="rId4"/>
     <sheet name="openAccount" sheetId="5" r:id="rId5"/>
     <sheet name="OneJN_TC1" sheetId="6" r:id="rId6"/>
+    <sheet name="testbox" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:S14"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>username</t>
   </si>
@@ -119,6 +119,51 @@
   </si>
   <si>
     <t>chanelle012</t>
+  </si>
+  <si>
+    <t>fullname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>curaddress</t>
+  </si>
+  <si>
+    <t>peraddress</t>
+  </si>
+  <si>
+    <t>Karun</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>singh@gmail.com</t>
+  </si>
+  <si>
+    <t>expfullname</t>
+  </si>
+  <si>
+    <t>expemail</t>
+  </si>
+  <si>
+    <t>expcuraddress</t>
+  </si>
+  <si>
+    <t>expperaddress</t>
+  </si>
+  <si>
+    <t>Name:Karun</t>
+  </si>
+  <si>
+    <t>Email:singh@gmail.com</t>
+  </si>
+  <si>
+    <t>Current Address :address</t>
+  </si>
+  <si>
+    <t>Permananet Address :peraddress</t>
   </si>
 </sst>
 </file>
@@ -473,7 +518,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -699,7 +744,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -727,4 +772,74 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>